<commit_message>
Finished the analysis of the outdoor ads (added qwen)
</commit_message>
<xml_diff>
--- a/data/gpt_all_outdoor.xlsx
+++ b/data/gpt_all_outdoor.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BG101"/>
+  <dimension ref="A1:BI101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -653,6 +653,16 @@
           <t>processed_explanation_16</t>
         </is>
       </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>new_type_ad</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>new_who_cat</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -748,6 +758,16 @@
       <c r="S2">
         <v>34.46</v>
       </c>
+      <c r="BH2" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="BI2" t="inlineStr">
+        <is>
+          <t>A, NA</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -843,6 +863,16 @@
           <t>The food items are likely to be ultra-processed.</t>
         </is>
       </c>
+      <c r="BH3" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI3" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -958,6 +988,16 @@
           <t>These items are processed.</t>
         </is>
       </c>
+      <c r="BH4" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI4" t="inlineStr">
+        <is>
+          <t>4e, 9, 14</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1063,6 +1103,16 @@
           <t>The meats are processed for preparation and serving.</t>
         </is>
       </c>
+      <c r="BH5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI5" t="inlineStr">
+        <is>
+          <t>9, 14</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1158,6 +1208,16 @@
           <t>The juice is a processed product.</t>
         </is>
       </c>
+      <c r="BH6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI6" t="inlineStr">
+        <is>
+          <t>4a</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1283,6 +1343,16 @@
           <t>The bread is processed as part of the burger.</t>
         </is>
       </c>
+      <c r="BH7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI7" t="inlineStr">
+        <is>
+          <t>8, 9, 11, 14</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1378,6 +1448,16 @@
           <t>The burger is a composite dish with processed ingredients.</t>
         </is>
       </c>
+      <c r="BH8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI8" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1473,6 +1553,16 @@
           <t>Fanta is a formulation of industrial ingredients.</t>
         </is>
       </c>
+      <c r="BH9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI9" t="inlineStr">
+        <is>
+          <t>4e</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1568,6 +1658,16 @@
           <t>Ice creams are ultra-processed foods.</t>
         </is>
       </c>
+      <c r="BH10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1663,6 +1763,16 @@
       <c r="S11">
         <v>46.94</v>
       </c>
+      <c r="BH11" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="BI11" t="inlineStr">
+        <is>
+          <t>A, NA</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1788,6 +1898,16 @@
           <t>The vegetables appear fresh.</t>
         </is>
       </c>
+      <c r="BH12" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI12" t="inlineStr">
+        <is>
+          <t>8, 9, 13, 15</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1883,6 +2003,16 @@
       <c r="S13">
         <v>37.57</v>
       </c>
+      <c r="BH13" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="BI13" t="inlineStr">
+        <is>
+          <t>A, NA</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1978,6 +2108,16 @@
           <t>Soft drinks are typically ultra-processed.</t>
         </is>
       </c>
+      <c r="BH14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI14" t="inlineStr">
+        <is>
+          <t>4e</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2063,6 +2203,16 @@
       <c r="S15">
         <v>44.08</v>
       </c>
+      <c r="BH15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI15" t="inlineStr">
+        <is>
+          <t>4d</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2158,6 +2308,16 @@
           <t>The drink is a flavored carbonated beverage.</t>
         </is>
       </c>
+      <c r="BH16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI16" t="inlineStr">
+        <is>
+          <t>4e</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2243,6 +2403,16 @@
       <c r="S17">
         <v>36.04</v>
       </c>
+      <c r="BH17" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="BI17" t="inlineStr">
+        <is>
+          <t>A, 4f</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2338,6 +2508,16 @@
           <t>Kapsalon is a composite dish with multiple processed ingredients.</t>
         </is>
       </c>
+      <c r="BH18" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI18" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2433,6 +2613,16 @@
       <c r="S19">
         <v>37.94</v>
       </c>
+      <c r="BH19" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="BI19" t="inlineStr">
+        <is>
+          <t>A, NA</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2538,6 +2728,16 @@
           <t>Ice cream is a formulation of industrial ingredients.</t>
         </is>
       </c>
+      <c r="BH20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI20" t="inlineStr">
+        <is>
+          <t>5, 9</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2653,6 +2853,16 @@
           <t>These are fresh meat products.</t>
         </is>
       </c>
+      <c r="BH21" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BI21" t="inlineStr">
+        <is>
+          <t>9, 13, 14</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2758,6 +2968,16 @@
           <t>The Köfte is a processed meat product.</t>
         </is>
       </c>
+      <c r="BH22" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI22" t="inlineStr">
+        <is>
+          <t>9, 14</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2863,6 +3083,16 @@
           <t>Coffee is a processed beverage.</t>
         </is>
       </c>
+      <c r="BH23" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI23" t="inlineStr">
+        <is>
+          <t>4f, 9</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2958,6 +3188,16 @@
       <c r="S24">
         <v>45.98</v>
       </c>
+      <c r="BH24" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="BI24" t="inlineStr">
+        <is>
+          <t>A, NA</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3053,6 +3293,16 @@
           <t>Coca-Cola is an ultra-processed beverage.</t>
         </is>
       </c>
+      <c r="BH25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI25" t="inlineStr">
+        <is>
+          <t>4e</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3158,6 +3408,16 @@
           <t>Processed meats in burgers are typically ultra-processed.</t>
         </is>
       </c>
+      <c r="BH26" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI26" t="inlineStr">
+        <is>
+          <t>9, 14</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3273,6 +3533,16 @@
           <t>Fresh vegetables are minimally processed.</t>
         </is>
       </c>
+      <c r="BH27" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI27" t="inlineStr">
+        <is>
+          <t>9, 13, 15</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3368,6 +3638,16 @@
       <c r="S28">
         <v>33.05</v>
       </c>
+      <c r="BH28" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="BI28" t="inlineStr">
+        <is>
+          <t>A, NA</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3473,6 +3753,16 @@
           <t>The water is minimally processed.</t>
         </is>
       </c>
+      <c r="BH29" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI29" t="inlineStr">
+        <is>
+          <t>4f, 9</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3568,6 +3858,16 @@
           <t>Bread is typically processed through baking.</t>
         </is>
       </c>
+      <c r="BH30" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="BI30" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3673,6 +3973,16 @@
           <t>Falafel is made from processed chickpeas and spices.</t>
         </is>
       </c>
+      <c r="BH31" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI31" t="inlineStr">
+        <is>
+          <t>9, 17</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3768,6 +4078,16 @@
           <t>Coca-Cola is an ultra-processed beverage.</t>
         </is>
       </c>
+      <c r="BH32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI32" t="inlineStr">
+        <is>
+          <t>4e</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3883,6 +4203,16 @@
           <t>Pizza sauce is typically processed.</t>
         </is>
       </c>
+      <c r="BH33" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI33" t="inlineStr">
+        <is>
+          <t>9, 14, 18</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3978,6 +4308,16 @@
           <t>Tea is generally minimally processed.</t>
         </is>
       </c>
+      <c r="BH34" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BI34" t="inlineStr">
+        <is>
+          <t>4f</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4073,6 +4413,16 @@
       <c r="S35">
         <v>37.92</v>
       </c>
+      <c r="BH35" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="BI35" t="inlineStr">
+        <is>
+          <t>A, NA</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4168,6 +4518,16 @@
           <t>The drinks are flavored and bottled, indicating ultra-processing.</t>
         </is>
       </c>
+      <c r="BH36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI36" t="inlineStr">
+        <is>
+          <t>4e</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4263,6 +4623,16 @@
       <c r="S37">
         <v>40.06</v>
       </c>
+      <c r="BH37" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="BI37" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4358,6 +4728,16 @@
       <c r="S38">
         <v>13.31</v>
       </c>
+      <c r="BH38" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="BI38" t="inlineStr">
+        <is>
+          <t>A, NA</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4463,6 +4843,16 @@
           <t>Kebabs are considered processed due to the preparation methods.</t>
         </is>
       </c>
+      <c r="BH39" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI39" t="inlineStr">
+        <is>
+          <t>9, 14</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4558,6 +4948,16 @@
           <t>The pastry is likely processed.</t>
         </is>
       </c>
+      <c r="BH40" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI40" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4653,6 +5053,16 @@
           <t>Energy drinks are typically ultra-processed.</t>
         </is>
       </c>
+      <c r="BH41" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI41" t="inlineStr">
+        <is>
+          <t>4d</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4748,6 +5158,16 @@
       <c r="S42">
         <v>38.57</v>
       </c>
+      <c r="BH42" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="BI42" t="inlineStr">
+        <is>
+          <t>A, NA</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -4843,6 +5263,16 @@
       <c r="S43">
         <v>39.25</v>
       </c>
+      <c r="BH43" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="BI43" t="inlineStr">
+        <is>
+          <t>A, NA</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -4938,6 +5368,16 @@
           <t>The strawberries are fresh and unprocessed.</t>
         </is>
       </c>
+      <c r="BH44" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BI44" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -5053,6 +5493,16 @@
           <t>The pastries are likely processed.</t>
         </is>
       </c>
+      <c r="BH45" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BI45" t="inlineStr">
+        <is>
+          <t>2, 4f, 9</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5158,6 +5608,16 @@
           <t>These are industrially processed chocolate products.</t>
         </is>
       </c>
+      <c r="BH46" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI46" t="inlineStr">
+        <is>
+          <t>1, 5</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -5263,6 +5723,16 @@
           <t>Pastries are typically processed foods.</t>
         </is>
       </c>
+      <c r="BH47" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="BI47" t="inlineStr">
+        <is>
+          <t>2, 15</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -5368,6 +5838,16 @@
           <t>The seafood dishes are prepared and ready to eat.</t>
         </is>
       </c>
+      <c r="BH48" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI48" t="inlineStr">
+        <is>
+          <t>9, 14</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -5463,6 +5943,16 @@
           <t>The bread is a processed food item.</t>
         </is>
       </c>
+      <c r="BH49" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="BI49" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -5558,6 +6048,16 @@
           <t>Ice cream is a formulation of industrial ingredients.</t>
         </is>
       </c>
+      <c r="BH50" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI50" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -5653,6 +6153,16 @@
           <t>Soft drinks are formulations of industrial ingredients.</t>
         </is>
       </c>
+      <c r="BH51" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI51" t="inlineStr">
+        <is>
+          <t>4e</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -5748,6 +6258,16 @@
           <t>Ice creams are ultra-processed foods.</t>
         </is>
       </c>
+      <c r="BH52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI52" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -5843,6 +6363,16 @@
       <c r="S53">
         <v>24.27</v>
       </c>
+      <c r="BH53" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="BI53" t="inlineStr">
+        <is>
+          <t>A, NA</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -5938,6 +6468,16 @@
           <t>Energy drinks are typically ultra-processed due to added ingredients and industrial processing.</t>
         </is>
       </c>
+      <c r="BH54" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI54" t="inlineStr">
+        <is>
+          <t>4d</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -6033,6 +6573,16 @@
           <t>Coca-Cola is an ultra-processed beverage.</t>
         </is>
       </c>
+      <c r="BH55" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI55" t="inlineStr">
+        <is>
+          <t>4e</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -6128,6 +6678,16 @@
           <t>Energy drinks are typically ultra-processed.</t>
         </is>
       </c>
+      <c r="BH56" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI56" t="inlineStr">
+        <is>
+          <t>4d</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -6233,6 +6793,16 @@
           <t>The ice cream is a formulation of industrial ingredients.</t>
         </is>
       </c>
+      <c r="BH57" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI57" t="inlineStr">
+        <is>
+          <t>1, 5</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -6328,6 +6898,16 @@
       <c r="S58">
         <v>44.97</v>
       </c>
+      <c r="BH58" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="BI58" t="inlineStr">
+        <is>
+          <t>A, NA</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -6423,6 +7003,16 @@
       <c r="S59">
         <v>33.62</v>
       </c>
+      <c r="BH59" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="BI59" t="inlineStr">
+        <is>
+          <t>A, NA</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -6528,6 +7118,16 @@
           <t>The meat is likely seasoned and cooked, involving processing.</t>
         </is>
       </c>
+      <c r="BH60" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI60" t="inlineStr">
+        <is>
+          <t>9, 14</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -6623,6 +7223,16 @@
           <t>The cake and icing are processed food items.</t>
         </is>
       </c>
+      <c r="BH61" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="BI61" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -6728,6 +7338,16 @@
           <t>Bread is considered processed due to baking and ingredient combination.</t>
         </is>
       </c>
+      <c r="BH62" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI62" t="inlineStr">
+        <is>
+          <t>9, 11</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -6833,6 +7453,16 @@
           <t>The items like cakes and pastries are processed foods.</t>
         </is>
       </c>
+      <c r="BH63" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="BI63" t="inlineStr">
+        <is>
+          <t>2, 11</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -6928,6 +7558,16 @@
           <t>Pancakes are a processed food item.</t>
         </is>
       </c>
+      <c r="BH64" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI64" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -7023,6 +7663,16 @@
           <t>Pancakes are a processed food item.</t>
         </is>
       </c>
+      <c r="BH65" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI65" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -7128,6 +7778,16 @@
           <t>The spareribs are marinated, indicating processing.</t>
         </is>
       </c>
+      <c r="BH66" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI66" t="inlineStr">
+        <is>
+          <t>9, 14</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -7223,6 +7883,16 @@
       <c r="S67">
         <v>38.45</v>
       </c>
+      <c r="BH67" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="BI67" t="inlineStr">
+        <is>
+          <t>A, NA</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -7318,6 +7988,16 @@
           <t>The chips are an ultra-processed food product.</t>
         </is>
       </c>
+      <c r="BH68" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI68" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -7413,6 +8093,16 @@
           <t>The sandwich is a ready-made food item.</t>
         </is>
       </c>
+      <c r="BH69" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI69" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -7518,6 +8208,16 @@
           <t>The latte is a processed beverage.</t>
         </is>
       </c>
+      <c r="BH70" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI70" t="inlineStr">
+        <is>
+          <t>4b, 15</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -7613,6 +8313,16 @@
           <t>The omelet is a processed food item.</t>
         </is>
       </c>
+      <c r="BH71" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI71" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -7708,6 +8418,16 @@
       <c r="S72">
         <v>46.88</v>
       </c>
+      <c r="BH72" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="BI72" t="inlineStr">
+        <is>
+          <t>A, NA</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -7803,6 +8523,16 @@
       <c r="S73">
         <v>31.01</v>
       </c>
+      <c r="BH73" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="BI73" t="inlineStr">
+        <is>
+          <t>A, NA</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -7908,6 +8638,16 @@
           <t>The vegetables appear fresh and unprocessed.</t>
         </is>
       </c>
+      <c r="BH74" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI74" t="inlineStr">
+        <is>
+          <t>9, 15</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -8003,6 +8743,16 @@
       <c r="S75">
         <v>34.81</v>
       </c>
+      <c r="BH75" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="BI75" t="inlineStr">
+        <is>
+          <t>A, NA</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -8108,6 +8858,16 @@
           <t>The ice cream is a formulation of industrial ingredients.</t>
         </is>
       </c>
+      <c r="BH76" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI76" t="inlineStr">
+        <is>
+          <t>1, 5</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -8203,6 +8963,16 @@
       <c r="S77">
         <v>30.7</v>
       </c>
+      <c r="BH77" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="BI77" t="inlineStr">
+        <is>
+          <t>A, NA</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -8308,6 +9078,16 @@
           <t>The plant-based milk drink is likely ultra-processed due to industrial processing.</t>
         </is>
       </c>
+      <c r="BH78" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI78" t="inlineStr">
+        <is>
+          <t>1, 4c</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -8413,6 +9193,16 @@
           <t>Pastries are typically processed foods.</t>
         </is>
       </c>
+      <c r="BH79" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI79" t="inlineStr">
+        <is>
+          <t>2, 5</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -8508,6 +9298,16 @@
           <t>The chocolate is a formulated product.</t>
         </is>
       </c>
+      <c r="BH80" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI80" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -8603,6 +9403,16 @@
           <t>Pasta is a processed food product.</t>
         </is>
       </c>
+      <c r="BH81" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BI81" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -8698,6 +9508,16 @@
           <t>Cakes and pastries are typically processed foods.</t>
         </is>
       </c>
+      <c r="BH82" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="BI82" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -8793,6 +9613,16 @@
       <c r="S83">
         <v>36.22</v>
       </c>
+      <c r="BH83" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BI83" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -8888,6 +9718,16 @@
           <t>The applesauce is a processed fruit product.</t>
         </is>
       </c>
+      <c r="BH84" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BI84" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -8983,6 +9823,16 @@
           <t>Soft drinks are typically ultra-processed.</t>
         </is>
       </c>
+      <c r="BH85" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI85" t="inlineStr">
+        <is>
+          <t>4e</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -9078,6 +9928,16 @@
           <t>Ice cream is typically considered ultra-processed due to added sugars, flavors, and preservatives.</t>
         </is>
       </c>
+      <c r="BH86" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI86" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -9173,6 +10033,16 @@
           <t>The soft drink is an industrial formulation with additives.</t>
         </is>
       </c>
+      <c r="BH87" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI87" t="inlineStr">
+        <is>
+          <t>4e</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -9308,6 +10178,16 @@
           <t>Fries are typically processed through frying.</t>
         </is>
       </c>
+      <c r="BH88" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI88" t="inlineStr">
+        <is>
+          <t>3, 8, 9, 14, 18</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -9423,6 +10303,16 @@
           <t>The tartar sauce is a processed condiment.</t>
         </is>
       </c>
+      <c r="BH89" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI89" t="inlineStr">
+        <is>
+          <t>9, 14, 18</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -9518,6 +10408,16 @@
           <t>The meatballs are likely processed as they are part of a restaurant menu.</t>
         </is>
       </c>
+      <c r="BH90" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI90" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -9613,6 +10513,16 @@
           <t>The bread is a processed food item.</t>
         </is>
       </c>
+      <c r="BH91" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="BI91" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -9708,6 +10618,16 @@
           <t>The drink is likely a formulation of industrial ingredients.</t>
         </is>
       </c>
+      <c r="BH92" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI92" t="inlineStr">
+        <is>
+          <t>4e</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -9833,6 +10753,16 @@
           <t>Fresh vegetables are considered unprocessed foods.</t>
         </is>
       </c>
+      <c r="BH93" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI93" t="inlineStr">
+        <is>
+          <t>9, 11, 14, 15</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -9958,6 +10888,16 @@
           <t>Fries are typically processed.</t>
         </is>
       </c>
+      <c r="BH94" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI94" t="inlineStr">
+        <is>
+          <t>3, 4e, 9, 14</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -10083,6 +11023,16 @@
           <t>Fries are typically processed.</t>
         </is>
       </c>
+      <c r="BH95" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI95" t="inlineStr">
+        <is>
+          <t>3, 9, 11, 14</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -10188,6 +11138,16 @@
           <t>The drinks are processed with added ingredients.</t>
         </is>
       </c>
+      <c r="BH96" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI96" t="inlineStr">
+        <is>
+          <t>4b, 4f</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -10283,6 +11243,16 @@
           <t>Smoothies are processed as they are blended from fruits.</t>
         </is>
       </c>
+      <c r="BH97" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI97" t="inlineStr">
+        <is>
+          <t>4a</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -10398,6 +11368,16 @@
           <t>These are typically processed foods.</t>
         </is>
       </c>
+      <c r="BH98" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BI98" t="inlineStr">
+        <is>
+          <t>4e, 9, 14</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -10493,6 +11473,16 @@
           <t>Chocolate spreads are typically ultra-processed.</t>
         </is>
       </c>
+      <c r="BH99" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BI99" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -10588,6 +11578,16 @@
           <t>The cucumbers and corn appear fresh and unprocessed.</t>
         </is>
       </c>
+      <c r="BH100" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="BI100" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -10681,6 +11681,16 @@
       <c r="X101" t="inlineStr">
         <is>
           <t>Soft drinks are typically ultra-processed.</t>
+        </is>
+      </c>
+      <c r="BH101" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BI101" t="inlineStr">
+        <is>
+          <t>4e</t>
         </is>
       </c>
     </row>

</xml_diff>